<commit_message>
Add checker to hasil
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kerja\Projects\Cloudcakes\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{830AA14A-82AB-472D-BBA2-15C0F8BA9AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB771BF-93CD-46C4-BD2F-1D2734CDBC23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25065" yWindow="4065" windowWidth="16410" windowHeight="15345" xr2:uid="{D51E7D05-08E3-49A1-8F94-9E14D93A65D3}"/>
   </bookViews>
@@ -53,43 +53,43 @@
     <t>Darryl</t>
   </si>
   <si>
-    <t>Revan</t>
-  </si>
-  <si>
-    <t>revan.rile@gmail.com</t>
-  </si>
-  <si>
-    <t>darsryl.12032@gmail.com</t>
-  </si>
-  <si>
-    <t>Rezky</t>
-  </si>
-  <si>
-    <t>081867895569</t>
-  </si>
-  <si>
     <t>085653667887</t>
   </si>
   <si>
-    <t>rezky.ram@ymail.com</t>
-  </si>
-  <si>
-    <t>Yoril</t>
-  </si>
-  <si>
     <t>081312546455</t>
   </si>
   <si>
-    <t>yoril.yukan@gmail.com</t>
-  </si>
-  <si>
-    <t>Lukas</t>
-  </si>
-  <si>
     <t>085946556659</t>
   </si>
   <si>
-    <t>lukas.kenan@ymail.com</t>
+    <t>yoril baskara</t>
+  </si>
+  <si>
+    <t>reinaldi sianturi</t>
+  </si>
+  <si>
+    <t>reinald020@gmail.com</t>
+  </si>
+  <si>
+    <t>daryl2032@gmail.com</t>
+  </si>
+  <si>
+    <t>vincentius albert</t>
+  </si>
+  <si>
+    <t>albertvin9@gmail.com</t>
+  </si>
+  <si>
+    <t>zhaky hanif s.</t>
+  </si>
+  <si>
+    <t>081287892654</t>
+  </si>
+  <si>
+    <t>zhaky.hanif@yahoo.com</t>
+  </si>
+  <si>
+    <t>yoril.bass@yahoo.com</t>
   </si>
 </sst>
 </file>
@@ -477,7 +477,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,51 +506,51 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add check for false input
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kerja\Projects\Cloudcakes\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA665AF-E2FD-4691-BFAC-8D332CDDE475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B052880-A149-42CE-8F0A-C0847DC7C206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25065" yWindow="4065" windowWidth="16410" windowHeight="15345" xr2:uid="{D51E7D05-08E3-49A1-8F94-9E14D93A65D3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>name</t>
   </si>
@@ -108,6 +108,33 @@
   </si>
   <si>
     <t>kaniaa1993@gmail.com</t>
+  </si>
+  <si>
+    <t>paulus nugroho</t>
+  </si>
+  <si>
+    <t>087877589855</t>
+  </si>
+  <si>
+    <t>paulus.nug@yahoo.co.id</t>
+  </si>
+  <si>
+    <t>yudi bramanto</t>
+  </si>
+  <si>
+    <t>089989986746</t>
+  </si>
+  <si>
+    <t>yudiibram.78@gmail.com</t>
+  </si>
+  <si>
+    <t>levi prasetyo</t>
+  </si>
+  <si>
+    <t>087824656698</t>
+  </si>
+  <si>
+    <t>leviipras99@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -492,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{059AC859-59B7-49C1-908A-66A0CCC4A977}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,6 +620,39 @@
         <v>23</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{E5E7A5D0-4A8A-40F5-ABA4-860A5F03CEBD}"/>
@@ -602,6 +662,9 @@
     <hyperlink ref="C6" r:id="rId5" xr:uid="{36030F03-2D6D-4009-9425-90E049671223}"/>
     <hyperlink ref="C7" r:id="rId6" xr:uid="{3ACADEAA-95A8-4DB5-9CAA-4905E806C0C7}"/>
     <hyperlink ref="C8" r:id="rId7" xr:uid="{4B35FC6D-F0D1-4A0F-BF5B-6335F579CD93}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{D48FBC21-AC1B-45D9-AF66-BD04BBA6E817}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{26017F12-8CF1-47A6-92D6-7791885C2A50}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{AF307018-76CE-4D88-ABFC-C78D1ABFF3EA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>